<commit_message>
Rifatto contingency con case 3 giusto
</commit_message>
<xml_diff>
--- a/Provvisorio.xlsx
+++ b/Provvisorio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edoar\Desktop\UNI\A.A. 2025-2026\ELECTRIC POWER SYSTEM\progetto\ProgettoEPS1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10834079_polimi_it/Documents/Quarto anno/Primo semestre/EPS/Projects/Project 1 - Power Flow Analysis/ProgettoEPS1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE20972D-A79D-4283-9D77-17486600C767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{BE20972D-A79D-4283-9D77-17486600C767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E74AB93E-AC0D-4520-ADDD-7BADCF24268A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -6592,8 +6592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98F7985-A012-40CC-9F1A-039713B93512}">
   <dimension ref="B6:AQ274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G221" sqref="G221"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D238" sqref="D238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>